<commit_message>
publish as it stands after longtime
</commit_message>
<xml_diff>
--- a/REQUIREMENTS.xlsx
+++ b/REQUIREMENTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktemi\code\dabo_bet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktemi\code\dabo_bet\dabo_bet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14EC4AA4-F5D9-4047-85A0-5C76451C4898}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F0AA65-19C9-4A30-8C01-47D53D53F6C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5556" activeTab="2" xr2:uid="{F52AC00E-70D8-479E-880D-384F29DAF6B0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5556" xr2:uid="{F52AC00E-70D8-479E-880D-384F29DAF6B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,16 +161,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF77A23C-9602-4E86-A9DE-5E435A903B08}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:H7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,68 +527,68 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="129.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
@@ -616,19 +616,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -645,9 +645,9 @@
       <c r="D2">
         <v>73</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45413</v>
+        <v>45603</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -663,9 +663,9 @@
       <c r="D3">
         <v>80</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <f ca="1">TODAY()</f>
-        <v>45413</v>
+        <v>45603</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -681,9 +681,9 @@
       <c r="D4">
         <v>70</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <f ca="1">TODAY()</f>
-        <v>45413</v>
+        <v>45603</v>
       </c>
     </row>
   </sheetData>
@@ -695,7 +695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13D9BAD-727B-4E99-9235-1843109DBAC6}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>